<commit_message>
Added chart to excel sheet & added comments documenting the code.
</commit_message>
<xml_diff>
--- a/5/labProgram/distance_log.csv.xlsx
+++ b/5/labProgram/distance_log.csv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushaly\Documents\lab5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushaly\Documents\Labs\ESSE2220-labs\5\labProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF38CD91-23D8-4E30-85D0-15C6FB96C930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53BAA3F-F177-4052-8EF5-4B120F4AB71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CF3320C5-A773-4078-AA9F-CFEDFB686F08}"/>
   </bookViews>
@@ -95,6 +95,1806 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Distance from Sensor</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distance_cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>13.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.98</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.39</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.6300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.77</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.88</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.29</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.41</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.0299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.52</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.48</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.48</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.65</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14.03</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14.32</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14.34</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.26</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15.31</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.63</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.44</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10.74</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11.36</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>11.33</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.43</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.45</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.17</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.24</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.74</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.27</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13.65</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.35</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10.77</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>13.16</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>14.04</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>15.27</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>20.05</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>16.84</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>18.96</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>19.02</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>19.66</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>21.22</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>20.91</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>20.94</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20.34</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>20.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>19.09</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>19.309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>19.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>14.96</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13.14</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>12.28</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>12.87</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10.54</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.15</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10.18</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.26</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.58</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.67</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3.58</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5.76</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5.53</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.88</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>14.35</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.19</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>13.13</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>16.89</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>16.84</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>18.46</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>19.41</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>17.14</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>16.57</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>15.57</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>12.54</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>14.04</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>7.04</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>7.58</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>6.42</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.23</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>7.02</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>9.6300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>11.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EFF5-4C26-AE26-E05A462D5195}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1519185871"/>
+        <c:axId val="1519186287"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1519185871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519186287"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1519186287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519185871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>23232</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3716</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>334537</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>79916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0B3738-29EB-4430-A8D7-54C29E9B9509}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,7 +2197,7 @@
   <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,5 +3280,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>